<commit_message>
Added README.md for Reptor project
Introduction and comprehensive documentation of Reptor - the PHPSpreadsheet based report generator has been added. This covers the project's overview, key features, installation instructions, and usage instructions. The aim is to provide guidance for potential users or contributors to the project, making it easier to understand the purpose and functioning of Reptor.
</commit_message>
<xml_diff>
--- a/reports/sample-1-report.xlsx
+++ b/reports/sample-1-report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>Partner</t>
   </si>
@@ -73,15 +73,12 @@
     <t xml:space="preserve">Main street office </t>
   </si>
   <si>
-    <t>Main street office  összesen:</t>
+    <t>Main street office  sum:</t>
   </si>
   <si>
     <t>Dori Ann Gray</t>
   </si>
   <si>
-    <t>End of report</t>
-  </si>
-  <si>
     <t>Natalie D. Andie</t>
   </si>
   <si>
@@ -103,7 +100,7 @@
     <t xml:space="preserve">26 Diego al Mightie street </t>
   </si>
   <si>
-    <t>26 Diego al Mightie street  összesen:</t>
+    <t>26 Diego al Mightie street  sum:</t>
   </si>
   <si>
     <t>Ernesto di Scusting</t>
@@ -143,9 +140,6 @@
   </si>
   <si>
     <t>Alessio Stephard Ltd.</t>
-  </si>
-  <si>
-    <t>Alessio Stephard Ltd. összesen:</t>
   </si>
   <si>
     <t>Alessio Stephard Ltd. sum:</t>
@@ -224,7 +218,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,12 +229,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFBF819E"/>
         <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE0C2CD"/>
-        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -256,10 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="14">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
       <protection locked="true" hidden="false"/>
     </xf>
@@ -272,9 +257,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
       <protection locked="true" hidden="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
@@ -290,6 +272,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
       <protection locked="true" hidden="false"/>
     </xf>
@@ -303,9 +288,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="165" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="true">
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -607,238 +589,188 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AMJ41"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" showGridLines="true" showRowColHeaders="1" topLeftCell="A1">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A1">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="11.640625" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="11.53515625" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="31.66" customWidth="true" style="0"/>
-    <col min="2" max="2" width="27.78" customWidth="true" style="0"/>
-    <col min="3" max="3" width="30.1" customWidth="true" style="1"/>
-    <col min="6" max="6" width="16.67" customWidth="true" style="0"/>
-    <col min="7" max="7" width="15.15" customWidth="true" style="0"/>
-    <col min="9" max="9" width="15.41" customWidth="true" style="0"/>
-    <col min="10" max="10" width="14.28" customWidth="true" style="0"/>
-    <col min="974" max="974" width="11.52" customWidth="true" style="0"/>
-    <col min="975" max="975" width="11.52" customWidth="true" style="0"/>
-    <col min="976" max="976" width="11.52" customWidth="true" style="0"/>
-    <col min="977" max="977" width="11.52" customWidth="true" style="0"/>
-    <col min="978" max="978" width="11.52" customWidth="true" style="0"/>
-    <col min="979" max="979" width="11.52" customWidth="true" style="0"/>
-    <col min="980" max="980" width="11.52" customWidth="true" style="0"/>
-    <col min="981" max="981" width="11.52" customWidth="true" style="0"/>
-    <col min="982" max="982" width="11.52" customWidth="true" style="0"/>
-    <col min="983" max="983" width="11.52" customWidth="true" style="0"/>
-    <col min="984" max="984" width="11.52" customWidth="true" style="0"/>
-    <col min="985" max="985" width="11.52" customWidth="true" style="0"/>
-    <col min="986" max="986" width="11.52" customWidth="true" style="0"/>
-    <col min="987" max="987" width="11.52" customWidth="true" style="0"/>
-    <col min="988" max="988" width="11.52" customWidth="true" style="0"/>
-    <col min="989" max="989" width="11.52" customWidth="true" style="0"/>
-    <col min="990" max="990" width="11.52" customWidth="true" style="0"/>
-    <col min="991" max="991" width="11.52" customWidth="true" style="0"/>
-    <col min="992" max="992" width="11.52" customWidth="true" style="0"/>
-    <col min="993" max="993" width="11.52" customWidth="true" style="0"/>
-    <col min="994" max="994" width="11.52" customWidth="true" style="0"/>
-    <col min="995" max="995" width="11.52" customWidth="true" style="0"/>
-    <col min="996" max="996" width="11.52" customWidth="true" style="0"/>
-    <col min="997" max="997" width="11.52" customWidth="true" style="0"/>
-    <col min="998" max="998" width="11.52" customWidth="true" style="0"/>
-    <col min="999" max="999" width="11.52" customWidth="true" style="0"/>
-    <col min="1000" max="1000" width="11.52" customWidth="true" style="0"/>
-    <col min="1001" max="1001" width="11.52" customWidth="true" style="0"/>
-    <col min="1002" max="1002" width="11.52" customWidth="true" style="0"/>
-    <col min="1003" max="1003" width="11.52" customWidth="true" style="0"/>
-    <col min="1004" max="1004" width="11.52" customWidth="true" style="0"/>
-    <col min="1005" max="1005" width="11.52" customWidth="true" style="0"/>
-    <col min="1006" max="1006" width="11.52" customWidth="true" style="0"/>
-    <col min="1007" max="1007" width="11.52" customWidth="true" style="0"/>
-    <col min="1008" max="1008" width="11.52" customWidth="true" style="0"/>
-    <col min="1009" max="1009" width="11.52" customWidth="true" style="0"/>
-    <col min="1010" max="1010" width="11.52" customWidth="true" style="0"/>
-    <col min="1011" max="1011" width="11.52" customWidth="true" style="0"/>
-    <col min="1012" max="1012" width="11.52" customWidth="true" style="0"/>
-    <col min="1013" max="1013" width="11.52" customWidth="true" style="0"/>
-    <col min="1014" max="1014" width="11.52" customWidth="true" style="0"/>
-    <col min="1015" max="1015" width="11.52" customWidth="true" style="0"/>
-    <col min="1016" max="1016" width="11.52" customWidth="true" style="0"/>
-    <col min="1017" max="1017" width="11.52" customWidth="true" style="0"/>
-    <col min="1018" max="1018" width="11.52" customWidth="true" style="0"/>
-    <col min="1019" max="1019" width="11.52" customWidth="true" style="0"/>
-    <col min="1020" max="1020" width="11.52" customWidth="true" style="0"/>
-    <col min="1021" max="1021" width="11.52" customWidth="true" style="0"/>
-    <col min="1022" max="1022" width="11.52" customWidth="true" style="0"/>
-    <col min="1023" max="1023" width="11.52" customWidth="true" style="0"/>
-    <col min="1024" max="1024" width="11.52" customWidth="true" style="0"/>
+    <col min="1" max="1" width="28.06" customWidth="true" style="0"/>
+    <col min="2" max="2" width="23.89" customWidth="true" style="0"/>
+    <col min="3" max="3" width="29.03" customWidth="true" style="0"/>
+    <col min="6" max="6" width="15.28" customWidth="true" style="0"/>
+    <col min="7" max="7" width="18.47" customWidth="true" style="0"/>
+    <col min="8" max="8" width="15.14" customWidth="true" style="0"/>
+    <col min="9" max="9" width="14.16" customWidth="true" style="0"/>
+    <col min="10" max="10" width="15.97" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" customHeight="1" ht="35.95" s="5" customFormat="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:15" customHeight="1" ht="35.05">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-    </row>
-    <row r="2" spans="1:1024" customHeight="1" ht="12.8">
-      <c r="A2" s="2" t="s">
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" customHeight="1" ht="12.8">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="6">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="4">
         <v>3021</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="4">
         <v>1279</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="4">
         <v>196</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="4">
         <v>95</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="5">
         <v>0.48469387755102</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="4">
         <v>57</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="4">
         <v>86</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="4">
         <v>801</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="6">
         <v>74980499</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="4">
         <v>155.391</v>
       </c>
     </row>
-    <row r="3" spans="1:1024" customHeight="1" ht="35.95">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:15" customHeight="1" ht="46.25">
+      <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3"/>
-      <c r="D3" s="6">
+      <c r="C3" s="8"/>
+      <c r="D3" s="4">
         <v>3012</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>1276</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <v>146</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="4">
         <v>84</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="5">
         <f>G3/F3</f>
         <v>0.57534246575342</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="4">
         <v>35</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="4">
         <v>75</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="4">
         <v>746</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="6">
         <v>54846119</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="4">
         <v>135.391</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" customHeight="1" ht="31.7">
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="1:15" customHeight="1" ht="21.6">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>1225</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>745</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>7</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>4</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="5">
         <f>G4/F4</f>
         <v>0.57142857142857</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="4">
         <v>3</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="4">
         <v>4</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="4">
         <v>34</v>
       </c>
-      <c r="L4" s="8">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C5" s="11" t="s">
+    <row r="5" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>697</v>
       </c>
       <c r="E5">
@@ -850,7 +782,7 @@
       <c r="G5">
         <v>4</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <v>0.8</v>
       </c>
       <c r="I5">
@@ -862,18 +794,18 @@
       <c r="K5">
         <v>7</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="13">
         <v>0</v>
       </c>
       <c r="M5">
         <v>10.0</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="12">
+    <row r="6" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="11">
         <v>24</v>
       </c>
       <c r="E6">
@@ -885,7 +817,7 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="12">
         <v>0.0</v>
       </c>
       <c r="I6">
@@ -897,20 +829,16 @@
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="13">
         <v>0</v>
       </c>
       <c r="M6"/>
     </row>
-    <row r="7" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="A7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="12">
+    <row r="7" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="11">
         <v>0</v>
       </c>
       <c r="E7">
@@ -922,7 +850,7 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="12">
         <v>0.0</v>
       </c>
       <c r="I7">
@@ -934,20 +862,18 @@
       <c r="K7">
         <v>19</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="13">
         <v>0</v>
       </c>
       <c r="M7">
         <v>10.0</v>
       </c>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-    </row>
-    <row r="8" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="12">
+    </row>
+    <row r="8" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="11">
         <v>63</v>
       </c>
       <c r="E8">
@@ -959,7 +885,7 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="12">
         <v>0.0</v>
       </c>
       <c r="I8">
@@ -971,16 +897,16 @@
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="13">
         <v>0</v>
       </c>
       <c r="M8"/>
     </row>
-    <row r="9" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="12">
+    <row r="9" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="11">
         <v>207</v>
       </c>
       <c r="E9">
@@ -992,7 +918,7 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="12">
         <v>0.0</v>
       </c>
       <c r="I9">
@@ -1004,16 +930,16 @@
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="13">
         <v>0</v>
       </c>
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="12">
+    <row r="10" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="11">
         <v>3</v>
       </c>
       <c r="E10">
@@ -1025,7 +951,7 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="12">
         <v>0.0</v>
       </c>
       <c r="I10">
@@ -1037,17 +963,17 @@
       <c r="K10">
         <v>7</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="13">
         <v>0</v>
       </c>
       <c r="M10"/>
     </row>
-    <row r="11" spans="1:1024" customHeight="1" ht="19.9">
+    <row r="11" spans="1:15" customHeight="1" ht="12.8">
       <c r="B11"/>
-      <c r="C11" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="12">
+      <c r="C11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="11">
         <v>231</v>
       </c>
       <c r="E11">
@@ -1059,7 +985,7 @@
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="12">
         <v>0.0</v>
       </c>
       <c r="I11">
@@ -1071,57 +997,57 @@
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="13">
         <v>0</v>
       </c>
       <c r="M11">
         <v>10.0</v>
       </c>
     </row>
-    <row r="12" spans="1:1024" customHeight="1" ht="31.7">
-      <c r="B12" s="6" t="s">
+    <row r="12" spans="1:15" customHeight="1" ht="21.6">
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <v>1787</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <v>531</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="4">
         <v>139</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="4">
         <v>80</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="5">
         <f>G12/F12</f>
         <v>0.57553956834532</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="4">
         <v>32</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="4">
         <v>71</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="4">
         <v>712</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="6">
         <v>54846119</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="4">
         <v>105.391</v>
       </c>
     </row>
-    <row r="13" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C13" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="12">
+    <row r="13" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="11">
         <v>0</v>
       </c>
       <c r="E13">
@@ -1133,7 +1059,7 @@
       <c r="G13">
         <v>6</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="12">
         <v>1.0</v>
       </c>
       <c r="I13">
@@ -1145,18 +1071,18 @@
       <c r="K13">
         <v>123</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="13">
         <v>3541700</v>
       </c>
       <c r="M13">
         <v>10.0</v>
       </c>
     </row>
-    <row r="14" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C14" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="12">
+    <row r="14" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="11">
         <v>37</v>
       </c>
       <c r="E14">
@@ -1168,7 +1094,7 @@
       <c r="G14">
         <v>18</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="12">
         <v>0.9</v>
       </c>
       <c r="I14">
@@ -1180,18 +1106,18 @@
       <c r="K14">
         <v>87</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="13">
         <v>3844671</v>
       </c>
       <c r="M14">
         <v>9.7931</v>
       </c>
     </row>
-    <row r="15" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C15" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="12">
+    <row r="15" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="11">
         <v>60</v>
       </c>
       <c r="E15">
@@ -1203,7 +1129,7 @@
       <c r="G15">
         <v>13</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="12">
         <v>0.6842</v>
       </c>
       <c r="I15">
@@ -1215,18 +1141,18 @@
       <c r="K15">
         <v>79</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="13">
         <v>4574748</v>
       </c>
       <c r="M15">
         <v>8.7895</v>
       </c>
     </row>
-    <row r="16" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C16" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="12">
+    <row r="16" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="11">
         <v>1214</v>
       </c>
       <c r="E16">
@@ -1238,7 +1164,7 @@
       <c r="G16">
         <v>7</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="12">
         <v>0.7</v>
       </c>
       <c r="I16">
@@ -1250,18 +1176,18 @@
       <c r="K16">
         <v>27</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="13">
         <v>0</v>
       </c>
       <c r="M16">
         <v>9.6</v>
       </c>
     </row>
-    <row r="17" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="12">
+    <row r="17" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="11">
         <v>1</v>
       </c>
       <c r="E17">
@@ -1273,7 +1199,7 @@
       <c r="G17">
         <v>4</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="12">
         <v>0.25</v>
       </c>
       <c r="I17">
@@ -1285,18 +1211,18 @@
       <c r="K17">
         <v>27</v>
       </c>
-      <c r="L17" s="14">
+      <c r="L17" s="13">
         <v>4372500</v>
       </c>
       <c r="M17">
         <v>9.6667</v>
       </c>
     </row>
-    <row r="18" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C18" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="12">
+    <row r="18" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="11">
         <v>348</v>
       </c>
       <c r="E18">
@@ -1308,7 +1234,7 @@
       <c r="G18">
         <v>1</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="12">
         <v>1.0</v>
       </c>
       <c r="I18">
@@ -1320,18 +1246,18 @@
       <c r="K18">
         <v>18</v>
       </c>
-      <c r="L18" s="14">
+      <c r="L18" s="13">
         <v>2232000</v>
       </c>
       <c r="M18">
         <v>10.0</v>
       </c>
     </row>
-    <row r="19" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C19" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="12">
+    <row r="19" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="11">
         <v>0</v>
       </c>
       <c r="E19">
@@ -1343,7 +1269,7 @@
       <c r="G19">
         <v>4</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="12">
         <v>0.8</v>
       </c>
       <c r="I19">
@@ -1355,18 +1281,18 @@
       <c r="K19">
         <v>17</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="13">
         <v>3728500</v>
       </c>
       <c r="M19">
         <v>9.5</v>
       </c>
     </row>
-    <row r="20" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C20" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="12">
+    <row r="20" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="11">
         <v>17</v>
       </c>
       <c r="E20">
@@ -1378,7 +1304,7 @@
       <c r="G20">
         <v>9</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="12">
         <v>0.5294</v>
       </c>
       <c r="I20">
@@ -1390,18 +1316,18 @@
       <c r="K20">
         <v>51</v>
       </c>
-      <c r="L20" s="14">
+      <c r="L20" s="13">
         <v>22894150</v>
       </c>
       <c r="M20">
         <v>8.1667</v>
       </c>
     </row>
-    <row r="21" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C21" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="12">
+    <row r="21" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C21" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="11">
         <v>30</v>
       </c>
       <c r="E21">
@@ -1413,7 +1339,7 @@
       <c r="G21">
         <v>0</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="12">
         <v>0.0</v>
       </c>
       <c r="I21">
@@ -1425,16 +1351,16 @@
       <c r="K21">
         <v>0</v>
       </c>
-      <c r="L21" s="14">
+      <c r="L21" s="13">
         <v>0</v>
       </c>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C22" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="12">
+    <row r="22" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C22" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="11">
         <v>11</v>
       </c>
       <c r="E22">
@@ -1446,7 +1372,7 @@
       <c r="G22">
         <v>14</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="12">
         <v>0.7368</v>
       </c>
       <c r="I22">
@@ -1458,18 +1384,18 @@
       <c r="K22">
         <v>96</v>
       </c>
-      <c r="L22" s="14">
+      <c r="L22" s="13">
         <v>3138600</v>
       </c>
       <c r="M22">
         <v>9.875</v>
       </c>
     </row>
-    <row r="23" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C23" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="12">
+    <row r="23" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="11">
         <v>38</v>
       </c>
       <c r="E23">
@@ -1481,7 +1407,7 @@
       <c r="G23">
         <v>1</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="12">
         <v>0.05</v>
       </c>
       <c r="I23">
@@ -1493,20 +1419,20 @@
       <c r="K23">
         <v>13</v>
       </c>
-      <c r="L23" s="14">
+      <c r="L23" s="13">
         <v>6178000</v>
       </c>
       <c r="M23">
         <v>10.0</v>
       </c>
     </row>
-    <row r="24" spans="1:1024" customHeight="1" ht="19.9">
+    <row r="24" spans="1:15" customHeight="1" ht="12.8">
       <c r="A24"/>
       <c r="B24"/>
-      <c r="C24" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="12">
+      <c r="C24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="11">
         <v>31</v>
       </c>
       <c r="E24">
@@ -1518,7 +1444,7 @@
       <c r="G24">
         <v>3</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="12">
         <v>0.5</v>
       </c>
       <c r="I24">
@@ -1530,96 +1456,96 @@
       <c r="K24">
         <v>174</v>
       </c>
-      <c r="L24" s="14">
+      <c r="L24" s="13">
         <v>341250</v>
       </c>
       <c r="M24">
         <v>10.0</v>
       </c>
     </row>
-    <row r="25" spans="1:1024" customHeight="1" ht="35.95">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:15" customHeight="1" ht="46.25">
+      <c r="A25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="6">
+      <c r="D25" s="4">
         <v>9</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="4">
         <v>3</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="4">
         <v>50</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="4">
         <v>11</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="5">
         <f>G25/F25</f>
         <v>0.22</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="4">
         <v>22</v>
       </c>
-      <c r="J25" s="6">
+      <c r="J25" s="4">
         <v>11</v>
       </c>
-      <c r="K25" s="6">
+      <c r="K25" s="4">
         <v>55</v>
       </c>
-      <c r="L25" s="8">
+      <c r="L25" s="6">
         <v>20134380</v>
       </c>
-      <c r="M25" s="7">
+      <c r="M25" s="5">
         <v>0.48469387755102</v>
       </c>
     </row>
-    <row r="26" spans="1:1024" customHeight="1" ht="31.7">
-      <c r="B26" s="6" t="s">
+    <row r="26" spans="1:15" customHeight="1" ht="21.6">
+      <c r="B26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="6">
+      <c r="D26" s="4">
         <v>9</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="4">
         <v>3</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="4">
         <v>50</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="4">
         <v>11</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="5">
         <f>G26/F26</f>
         <v>0.22</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="4">
         <v>22</v>
       </c>
-      <c r="J26" s="6">
+      <c r="J26" s="4">
         <v>11</v>
       </c>
-      <c r="K26" s="6">
+      <c r="K26" s="4">
         <v>55</v>
       </c>
-      <c r="L26" s="8">
+      <c r="L26" s="6">
         <v>20134380</v>
       </c>
-      <c r="M26" s="6">
+      <c r="M26" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C27" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="12">
+    <row r="27" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C27" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="11">
         <v>0</v>
       </c>
       <c r="E27">
@@ -1631,7 +1557,7 @@
       <c r="G27">
         <v>0</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="12">
         <v>0.0</v>
       </c>
       <c r="I27">
@@ -1643,148 +1569,148 @@
       <c r="K27">
         <v>2</v>
       </c>
-      <c r="L27" s="14">
+      <c r="L27" s="13">
         <v>0</v>
       </c>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C28" s="11" t="s">
+    <row r="28" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C28" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="11">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28" s="13">
+        <v>0</v>
+      </c>
+      <c r="M28"/>
+    </row>
+    <row r="29" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C29" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="11">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29" s="13">
+        <v>314392</v>
+      </c>
+      <c r="M29"/>
+    </row>
+    <row r="30" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C30" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="12">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28" s="13">
+      <c r="D30" s="11">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" s="12">
         <v>0.0</v>
       </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28" s="14">
-        <v>0</v>
-      </c>
-      <c r="M28"/>
-    </row>
-    <row r="29" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C29" s="11" t="s">
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30" s="13">
+        <v>0</v>
+      </c>
+      <c r="M30"/>
+    </row>
+    <row r="31" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C31" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="12">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29" s="13">
+      <c r="D31" s="11">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" s="12">
         <v>0.0</v>
       </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29" s="14">
-        <v>314392</v>
-      </c>
-      <c r="M29"/>
-    </row>
-    <row r="30" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C30" s="11" t="s">
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31" s="13">
+        <v>0</v>
+      </c>
+      <c r="M31"/>
+    </row>
+    <row r="32" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C32" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="12">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30" s="14">
-        <v>0</v>
-      </c>
-      <c r="M30"/>
-    </row>
-    <row r="31" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C31" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="12">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31" s="14">
-        <v>0</v>
-      </c>
-      <c r="M31"/>
-    </row>
-    <row r="32" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C32" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D32" s="12">
+      <c r="D32" s="11">
         <v>0</v>
       </c>
       <c r="E32">
@@ -1796,7 +1722,7 @@
       <c r="G32">
         <v>0</v>
       </c>
-      <c r="H32" s="13">
+      <c r="H32" s="12">
         <v>0.0</v>
       </c>
       <c r="I32">
@@ -1808,16 +1734,16 @@
       <c r="K32">
         <v>2</v>
       </c>
-      <c r="L32" s="14">
+      <c r="L32" s="13">
         <v>600000</v>
       </c>
       <c r="M32"/>
     </row>
-    <row r="33" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C33" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="12">
+    <row r="33" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C33" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="11">
         <v>9</v>
       </c>
       <c r="E33">
@@ -1829,7 +1755,7 @@
       <c r="G33">
         <v>4</v>
       </c>
-      <c r="H33" s="13">
+      <c r="H33" s="12">
         <v>0.2667</v>
       </c>
       <c r="I33">
@@ -1841,18 +1767,18 @@
       <c r="K33">
         <v>36</v>
       </c>
-      <c r="L33" s="14">
+      <c r="L33" s="13">
         <v>1774500</v>
       </c>
       <c r="M33">
         <v>10.0</v>
       </c>
     </row>
-    <row r="34" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C34" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="12">
+    <row r="34" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C34" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="11">
         <v>0</v>
       </c>
       <c r="E34">
@@ -1864,7 +1790,7 @@
       <c r="G34">
         <v>1</v>
       </c>
-      <c r="H34" s="13">
+      <c r="H34" s="12">
         <v>0.0833</v>
       </c>
       <c r="I34">
@@ -1876,117 +1802,117 @@
       <c r="K34">
         <v>10</v>
       </c>
-      <c r="L34" s="14">
+      <c r="L34" s="13">
         <v>17445488</v>
       </c>
       <c r="M34">
         <v>10.0</v>
       </c>
     </row>
-    <row r="35" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C35" s="11" t="s">
+    <row r="35" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C35" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="11">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35" s="13">
+        <v>0</v>
+      </c>
+      <c r="M35"/>
+    </row>
+    <row r="36" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C36" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="11">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36" s="13">
+        <v>0</v>
+      </c>
+      <c r="M36"/>
+    </row>
+    <row r="37" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C37" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="12">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35" s="13">
+      <c r="D37" s="11">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37" s="12">
         <v>0.0</v>
       </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35" s="14">
-        <v>0</v>
-      </c>
-      <c r="M35"/>
-    </row>
-    <row r="36" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C36" s="11" t="s">
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37" s="13">
+        <v>0</v>
+      </c>
+      <c r="M37"/>
+    </row>
+    <row r="38" spans="1:15" customHeight="1" ht="12.8">
+      <c r="C38" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="12">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36" s="14">
-        <v>0</v>
-      </c>
-      <c r="M36"/>
-    </row>
-    <row r="37" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C37" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D37" s="12">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <v>1</v>
-      </c>
-      <c r="L37" s="14">
-        <v>0</v>
-      </c>
-      <c r="M37"/>
-    </row>
-    <row r="38" spans="1:1024" customHeight="1" ht="19.9">
-      <c r="C38" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D38" s="12">
+      <c r="D38" s="11">
         <v>0</v>
       </c>
       <c r="E38">
@@ -1998,7 +1924,7 @@
       <c r="G38">
         <v>6</v>
       </c>
-      <c r="H38" s="13">
+      <c r="H38" s="12">
         <v>0.2727</v>
       </c>
       <c r="I38">
@@ -2010,25 +1936,10 @@
       <c r="K38">
         <v>3</v>
       </c>
-      <c r="L38" s="14">
+      <c r="L38" s="13">
         <v>0</v>
       </c>
       <c r="M38"/>
-    </row>
-    <row r="39" spans="1:1024" customHeight="1" ht="12.75"/>
-    <row r="40" spans="1:1024" customHeight="1" ht="12.75"/>
-    <row r="41" spans="1:1024" customHeight="1" ht="12.75">
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
     </row>
   </sheetData>
   <mergeCells>

</xml_diff>